<commit_message>
Update XLOOKUP tutorial file with new examples and enhancements
</commit_message>
<xml_diff>
--- a/Excel/XLOOKUP Excel Tutorial File.xlsx
+++ b/Excel/XLOOKUP Excel Tutorial File.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/579481080490e445/Documents/Excel Series Excels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\sql_practice\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{625F3FEF-17C5-43E2-BFC2-A4868BFCBA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C527314-E796-4D19-8242-2D39E262C562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5EA44D8F-79D3-45F5-A0F6-C7F47358B7ED}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="14586" firstSheet="3" activeTab="3" xr2:uid="{5EA44D8F-79D3-45F5-A0F6-C7F47358B7ED}"/>
   </bookViews>
   <sheets>
     <sheet name="XLookUp" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="93">
   <si>
     <t>EmployeeID</t>
   </si>
@@ -316,6 +316,9 @@
   </si>
   <si>
     <t>Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meredith </t>
   </si>
 </sst>
 </file>
@@ -373,9 +376,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -413,7 +416,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -519,7 +522,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -661,7 +664,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -671,19 +674,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1027015F-D30F-450C-928C-DE78480974B7}">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.05859375" customWidth="1"/>
+    <col min="2" max="2" width="24.52734375" customWidth="1"/>
+    <col min="8" max="8" width="14.64453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.76171875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="40.64453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.5">
       <c r="E1" t="s">
         <v>0</v>
       </c>
@@ -721,7 +725,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -762,10 +766,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>65</v>
       </c>
+      <c r="B3" t="str">
+        <f>_xlfn.XLOOKUP(A3,H1:H9,P1:P9,"Not Found",2)</f>
+        <v>Toby.Flenderson@DunderMifflinCorporate.com</v>
+      </c>
       <c r="E3">
         <v>1002</v>
       </c>
@@ -800,10 +808,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>62</v>
       </c>
+      <c r="B4" t="str">
+        <f>_xlfn.XLOOKUP(A4,H2:H10,P2:P10,"Not Found",2)</f>
+        <v>Pam.Beasley@DunderMifflin.com</v>
+      </c>
       <c r="E4">
         <v>1003</v>
       </c>
@@ -838,9 +850,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>92</v>
+      </c>
+      <c r="B5" t="str">
+        <f>_xlfn.XLOOKUP(A5,H3:H11,P3:P11,"Not Found",2)</f>
+        <v>Not Found</v>
       </c>
       <c r="E5">
         <v>1004</v>
@@ -876,10 +892,14 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>69</v>
       </c>
+      <c r="B6" t="str">
+        <f t="shared" ref="B5:B6" si="0">_xlfn.XLOOKUP(A6,H4:H12,P4:P12,"Not Found",2)</f>
+        <v>Kevin.Malone@DunderMifflin.com</v>
+      </c>
       <c r="E6">
         <v>1005</v>
       </c>
@@ -914,7 +934,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.5">
       <c r="E7">
         <v>1006</v>
       </c>
@@ -949,7 +969,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.5">
       <c r="E8">
         <v>1007</v>
       </c>
@@ -984,7 +1004,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.5">
       <c r="E9">
         <v>1008</v>
       </c>
@@ -1019,7 +1039,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.5">
       <c r="E10">
         <v>1009</v>
       </c>
@@ -1054,15 +1074,15 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="8:8" x14ac:dyDescent="0.5">
       <c r="H22" t="str">
-        <f t="shared" ref="H22:H23" si="0">CONCATENATE(F12," ",G12)</f>
+        <f t="shared" ref="H22:H23" si="1">CONCATENATE(F12," ",G12)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="8:8" x14ac:dyDescent="0.5">
       <c r="H23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -1073,57 +1093,58 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEFF05A7-3704-402E-8684-C856D6F82881}">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.64453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.52734375" customWidth="1"/>
+    <col min="7" max="7" width="9.1171875" customWidth="1"/>
+    <col min="8" max="8" width="14.64453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.76171875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="40.64453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
       <c r="F1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="I1" t="s">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="J1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -1133,341 +1154,354 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="F2">
+      <c r="E2">
         <v>1001</v>
       </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
       <c r="G2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J2">
+      <c r="I2">
         <v>30</v>
       </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
       <c r="K2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" t="s">
         <v>13</v>
       </c>
-      <c r="M2">
+      <c r="L2">
         <v>45000</v>
       </c>
+      <c r="M2" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="N2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>65</v>
       </c>
-      <c r="F3">
+      <c r="C3" t="str">
+        <f>_xlfn.XLOOKUP(A3,H3:H10,O3:O10,"Not Found",2)</f>
+        <v>Toby.Flenderson@DunderMifflinCorporate.com</v>
+      </c>
+      <c r="E3">
         <v>1002</v>
       </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I3">
+        <v>30</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3">
+        <v>36000</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="I3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J3">
-        <v>30</v>
-      </c>
-      <c r="K3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3">
-        <v>36000</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F4">
+      <c r="C4" t="str">
+        <f>_xlfn.XLOOKUP("*"&amp;A4,H4:H11,O4:O11,"Not Found",2)</f>
+        <v>Not Found</v>
+      </c>
+      <c r="E4">
         <v>1003</v>
       </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" t="s">
         <v>63</v>
       </c>
-      <c r="J4">
+      <c r="I4">
         <v>29</v>
       </c>
+      <c r="J4" t="s">
+        <v>12</v>
+      </c>
       <c r="K4" t="s">
-        <v>12</v>
-      </c>
-      <c r="L4" t="s">
         <v>13</v>
       </c>
-      <c r="M4">
+      <c r="L4">
         <v>63000</v>
       </c>
+      <c r="M4" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="N4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>67</v>
       </c>
-      <c r="F5">
+      <c r="C5" t="str">
+        <f t="shared" ref="C5:C6" si="0">_xlfn.XLOOKUP(A5&amp;"*",H5:H12,O5:O12,"Not Found",2)</f>
+        <v>Meredith.Palmer@Yahoo.com</v>
+      </c>
+      <c r="E5">
         <v>1004</v>
       </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" t="s">
         <v>64</v>
       </c>
-      <c r="J5">
+      <c r="I5">
         <v>31</v>
       </c>
+      <c r="J5" t="s">
+        <v>19</v>
+      </c>
       <c r="K5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" t="s">
         <v>31</v>
       </c>
-      <c r="M5">
+      <c r="L5">
         <v>47000</v>
       </c>
+      <c r="M5" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="N5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="O5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>69</v>
       </c>
-      <c r="F6">
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>Kevin.Malone@DunderMifflin.com</v>
+      </c>
+      <c r="E6">
         <v>1005</v>
       </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
       <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6">
+        <v>32</v>
+      </c>
+      <c r="J6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6">
+        <v>50000</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E7">
+        <v>1006</v>
+      </c>
+      <c r="F7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" t="s">
+        <v>66</v>
+      </c>
+      <c r="I7">
         <v>35</v>
       </c>
-      <c r="H6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" t="s">
-        <v>65</v>
-      </c>
-      <c r="J6">
+      <c r="J7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7">
+        <v>65000</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E8">
+        <v>1007</v>
+      </c>
+      <c r="F8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" t="s">
+        <v>67</v>
+      </c>
+      <c r="I8">
         <v>32</v>
       </c>
-      <c r="K6" t="s">
+      <c r="J8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L8">
+        <v>41000</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E9">
+        <v>1008</v>
+      </c>
+      <c r="F9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" t="s">
+        <v>68</v>
+      </c>
+      <c r="I9">
+        <v>38</v>
+      </c>
+      <c r="J9" t="s">
         <v>12</v>
       </c>
-      <c r="L6" t="s">
-        <v>37</v>
-      </c>
-      <c r="M6">
-        <v>50000</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F7">
-        <v>1006</v>
-      </c>
-      <c r="G7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" t="s">
-        <v>66</v>
-      </c>
-      <c r="J7">
-        <v>35</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="K9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9">
+        <v>48000</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E10">
+        <v>1009</v>
+      </c>
+      <c r="F10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10">
+        <v>31</v>
+      </c>
+      <c r="J10" t="s">
         <v>12</v>
       </c>
-      <c r="L7" t="s">
-        <v>43</v>
-      </c>
-      <c r="M7">
-        <v>65000</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F8">
-        <v>1007</v>
-      </c>
-      <c r="G8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" t="s">
-        <v>47</v>
-      </c>
-      <c r="I8" t="s">
-        <v>67</v>
-      </c>
-      <c r="J8">
-        <v>32</v>
-      </c>
-      <c r="K8" t="s">
-        <v>19</v>
-      </c>
-      <c r="L8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M8">
-        <v>41000</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F9">
-        <v>1008</v>
-      </c>
-      <c r="G9" t="s">
-        <v>51</v>
-      </c>
-      <c r="H9" t="s">
-        <v>52</v>
-      </c>
-      <c r="I9" t="s">
-        <v>68</v>
-      </c>
-      <c r="J9">
-        <v>38</v>
-      </c>
-      <c r="K9" t="s">
-        <v>12</v>
-      </c>
-      <c r="L9" t="s">
-        <v>13</v>
-      </c>
-      <c r="M9">
-        <v>48000</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="O9" s="1" t="s">
+      <c r="K10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10">
+        <v>42000</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="P9" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F10">
-        <v>1009</v>
-      </c>
-      <c r="G10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H10" t="s">
-        <v>57</v>
-      </c>
-      <c r="I10" t="s">
-        <v>69</v>
-      </c>
-      <c r="J10">
-        <v>31</v>
-      </c>
-      <c r="K10" t="s">
-        <v>12</v>
-      </c>
-      <c r="L10" t="s">
-        <v>31</v>
-      </c>
-      <c r="M10">
-        <v>42000</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="P10" s="2" t="s">
+      <c r="O10" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I22" t="str">
-        <f t="shared" ref="I22:I23" si="0">CONCATENATE(G12," ",H12)</f>
+    <row r="22" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H22" t="str">
+        <f t="shared" ref="H22:H23" si="1">CONCATENATE(F12," ",G12)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I23" t="str">
-        <f t="shared" si="0"/>
+    <row r="23" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H23" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -1481,19 +1515,19 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.64453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.52734375" customWidth="1"/>
+    <col min="8" max="8" width="14.64453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.76171875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="40.64453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.5">
       <c r="E1" t="s">
         <v>0</v>
       </c>
@@ -1528,7 +1562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -1569,10 +1603,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>86</v>
       </c>
+      <c r="B3" t="str">
+        <f>_xlfn.XLOOKUP(A3,H2:H10, O2:O10,"Not Found",1)</f>
+        <v>Toby.Flenderson@DunderMifflinCorporate.com</v>
+      </c>
       <c r="E3">
         <v>1002</v>
       </c>
@@ -1607,10 +1645,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>18</v>
       </c>
+      <c r="B4" t="str">
+        <f>_xlfn.XLOOKUP("*"&amp;A4,H3:H11, O3:O11,"Not Found",2)</f>
+        <v>Pam.Beasley@DunderMifflin.com</v>
+      </c>
       <c r="E4">
         <v>1003</v>
       </c>
@@ -1645,10 +1687,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>46</v>
       </c>
+      <c r="B5" t="str">
+        <f>_xlfn.XLOOKUP(A5&amp;"*",H4:H12, O4:O12,"Not Found",2)</f>
+        <v>Meredith.Palmer@Yahoo.com</v>
+      </c>
       <c r="E5">
         <v>1004</v>
       </c>
@@ -1683,10 +1729,14 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>87</v>
       </c>
+      <c r="B6" t="str">
+        <f t="shared" ref="B6:B7" si="0">_xlfn.XLOOKUP(A6&amp;"*",H5:H13, O5:O13,"Not Found",2)</f>
+        <v>Kevin.Malone@DunderMifflin.com</v>
+      </c>
       <c r="E6">
         <v>1005</v>
       </c>
@@ -1721,7 +1771,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.5">
       <c r="E7">
         <v>1006</v>
       </c>
@@ -1756,7 +1806,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.5">
       <c r="E8">
         <v>1007</v>
       </c>
@@ -1791,7 +1841,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.5">
       <c r="E9">
         <v>1008</v>
       </c>
@@ -1826,7 +1876,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.5">
       <c r="E10">
         <v>1009</v>
       </c>
@@ -1861,15 +1911,15 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="8:8" x14ac:dyDescent="0.5">
       <c r="H22" t="str">
-        <f t="shared" ref="H22:H23" si="0">CONCATENATE(F12," ",G12)</f>
+        <f t="shared" ref="H22:H23" si="1">CONCATENATE(F12," ",G12)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="8:8" x14ac:dyDescent="0.5">
       <c r="H23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -1882,21 +1932,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22A42832-12A0-41C9-BED0-20D277223524}">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.77734375" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.64453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.76171875" customWidth="1"/>
+    <col min="3" max="3" width="24.52734375" customWidth="1"/>
+    <col min="9" max="9" width="14.64453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.76171875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="40.64453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.5">
       <c r="F1" t="s">
         <v>0</v>
       </c>
@@ -1931,7 +1981,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -1972,10 +2022,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>90</v>
       </c>
+      <c r="B3" t="str">
+        <f>_xlfn.XLOOKUP(A3,N2:N10,I2:I10,,1)</f>
+        <v>Angela Martin</v>
+      </c>
       <c r="F3">
         <v>1002</v>
       </c>
@@ -2010,10 +2064,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="B4" t="str">
+        <f>_xlfn.XLOOKUP(A4,N3:N11,I3:I11,,,1)</f>
+        <v>Toby Flenderson</v>
+      </c>
       <c r="F4">
         <v>1003</v>
       </c>
@@ -2048,7 +2106,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.5">
       <c r="F5">
         <v>1004</v>
       </c>
@@ -2083,7 +2141,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.5">
       <c r="F6">
         <v>1005</v>
       </c>
@@ -2118,7 +2176,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.5">
       <c r="F7">
         <v>1006</v>
       </c>
@@ -2153,7 +2211,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.5">
       <c r="F8">
         <v>1007</v>
       </c>
@@ -2188,7 +2246,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.5">
       <c r="F9">
         <v>1008</v>
       </c>
@@ -2223,7 +2281,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.5">
       <c r="F10">
         <v>1009</v>
       </c>
@@ -2258,13 +2316,13 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="9:9" x14ac:dyDescent="0.5">
       <c r="I22" t="str">
         <f t="shared" ref="I22:I23" si="0">CONCATENATE(G12," ",H12)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="9:9" x14ac:dyDescent="0.5">
       <c r="I23" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
@@ -2283,12 +2341,12 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.5">
       <c r="B1" t="s">
         <v>73</v>
       </c>
@@ -2329,7 +2387,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -2373,7 +2431,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -2417,7 +2475,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -2474,12 +2532,12 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.5">
       <c r="B1" t="s">
         <v>73</v>
       </c>
@@ -2520,7 +2578,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -2564,7 +2622,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -2608,7 +2666,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -2652,12 +2710,12 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.5">
       <c r="B6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -2675,12 +2733,12 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.41015625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.5">
       <c r="E1" t="s">
         <v>0</v>
       </c>
@@ -2718,7 +2776,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -2759,7 +2817,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -2797,7 +2855,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -2835,7 +2893,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -2873,7 +2931,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.5">
       <c r="E6">
         <v>1005</v>
       </c>
@@ -2908,7 +2966,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.5">
       <c r="E7">
         <v>1006</v>
       </c>
@@ -2943,7 +3001,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.5">
       <c r="E8">
         <v>1007</v>
       </c>
@@ -2978,7 +3036,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.5">
       <c r="E9">
         <v>1008</v>
       </c>
@@ -3013,7 +3071,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.5">
       <c r="E10">
         <v>1009</v>
       </c>

</xml_diff>

<commit_message>
Add new Conditional Formatting tutorial file and update XLOOKUP tutorial file
</commit_message>
<xml_diff>
--- a/Excel/XLOOKUP Excel Tutorial File.xlsx
+++ b/Excel/XLOOKUP Excel Tutorial File.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\sql_practice\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C527314-E796-4D19-8242-2D39E262C562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9465E0-183A-4BA9-AA9D-7296E685364B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="14586" firstSheet="3" activeTab="3" xr2:uid="{5EA44D8F-79D3-45F5-A0F6-C7F47358B7ED}"/>
+    <workbookView xWindow="16213" yWindow="0" windowWidth="9467" windowHeight="14480" tabRatio="836" firstSheet="5" activeTab="6" xr2:uid="{5EA44D8F-79D3-45F5-A0F6-C7F47358B7ED}"/>
   </bookViews>
   <sheets>
     <sheet name="XLookUp" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="95">
   <si>
     <t>EmployeeID</t>
   </si>
@@ -319,6 +319,12 @@
   </si>
   <si>
     <t xml:space="preserve">Meredith </t>
+  </si>
+  <si>
+    <t xml:space="preserve">x  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -897,7 +903,7 @@
         <v>69</v>
       </c>
       <c r="B6" t="str">
-        <f t="shared" ref="B5:B6" si="0">_xlfn.XLOOKUP(A6,H4:H12,P4:P12,"Not Found",2)</f>
+        <f t="shared" ref="B6" si="0">_xlfn.XLOOKUP(A6,H4:H12,P4:P12,"Not Found",2)</f>
         <v>Kevin.Malone@DunderMifflin.com</v>
       </c>
       <c r="E6">
@@ -1096,7 +1102,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1274,7 +1280,7 @@
         <v>67</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" ref="C5:C6" si="0">_xlfn.XLOOKUP(A5&amp;"*",H5:H12,O5:O12,"Not Found",2)</f>
+        <f>_xlfn.XLOOKUP(A5&amp;"*",H5:H12,O5:O12,"Not Found",2)</f>
         <v>Meredith.Palmer@Yahoo.com</v>
       </c>
       <c r="E5">
@@ -1316,7 +1322,7 @@
         <v>69</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C5:C6" si="0">_xlfn.XLOOKUP(A6&amp;"*",H6:H13,O6:O13,"Not Found",2)</f>
         <v>Kevin.Malone@DunderMifflin.com</v>
       </c>
       <c r="E6">
@@ -1734,7 +1740,7 @@
         <v>87</v>
       </c>
       <c r="B6" t="str">
-        <f t="shared" ref="B6:B7" si="0">_xlfn.XLOOKUP(A6&amp;"*",H5:H13, O5:O13,"Not Found",2)</f>
+        <f t="shared" ref="B6" si="0">_xlfn.XLOOKUP(A6&amp;"*",H5:H13, O5:O13,"Not Found",2)</f>
         <v>Kevin.Malone@DunderMifflin.com</v>
       </c>
       <c r="E6">
@@ -1932,19 +1938,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22A42832-12A0-41C9-BED0-20D277223524}">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
-  <cols>
-    <col min="1" max="1" width="14.64453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.76171875" customWidth="1"/>
-    <col min="3" max="3" width="24.52734375" customWidth="1"/>
-    <col min="9" max="9" width="14.64453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.76171875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="40.64453125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="9.9375" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.5">
       <c r="F1" t="s">
@@ -2026,9 +2024,8 @@
       <c r="A3" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B3" t="str">
-        <f>_xlfn.XLOOKUP(A3,N2:N10,I2:I10,,1)</f>
-        <v>Angela Martin</v>
+      <c r="B3" t="s">
+        <v>93</v>
       </c>
       <c r="F3">
         <v>1002</v>
@@ -2528,8 +2525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A2549A4-3A41-4806-B7FD-3B9C6823775F}">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2719,6 +2716,10 @@
       <c r="A7" t="s">
         <v>70</v>
       </c>
+      <c r="B7">
+        <f>SUM(_xlfn.XLOOKUP(I1,H1:S1,H2:S2):_xlfn.XLOOKUP(J1,H1:S1,H2:S2))</f>
+        <v>460</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2729,8 +2730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8F9C169-12D8-441E-870D-6C6EF0F6521C}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -3072,6 +3073,9 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="C10" t="s">
+        <v>94</v>
+      </c>
       <c r="E10">
         <v>1009</v>
       </c>

</xml_diff>